<commit_message>
Fix unit test file of 57fedb272cfcad3436142dbe9eac2870e3c3e3d2
Change "Comic Sans MS" font type to "Calibri" of cell formats.

Change-Id: If29fd11fa0c79f243ba81d5ddc745692b8a3b25b
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/tdf134225.xlsx
+++ b/chart2/qa/extras/data/xlsx/tdf134225.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vargabalazs3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\balu\sources\core\chart2\qa\extras\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2435D16B-BEF2-4DEB-836C-C5343C7C1228}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7178C2-0842-485C-AE66-9B6705037277}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD9F8B00-C741-4F0F-A610-36CF13335972}"/>
+    <workbookView xWindow="6285" yWindow="4410" windowWidth="28800" windowHeight="15375" xr2:uid="{CD9F8B00-C741-4F0F-A610-36CF13335972}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -65,6 +65,14 @@
       <name val="Comic Sans MS"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -172,6 +181,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-FBD4-4A9D-9613-3FBB4E19AFCC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -187,6 +201,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-FBD4-4A9D-9613-3FBB4E19AFCC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -202,6 +221,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-FBD4-4A9D-9613-3FBB4E19AFCC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -217,6 +241,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-FBD4-4A9D-9613-3FBB4E19AFCC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -232,6 +261,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-FBD4-4A9D-9613-3FBB4E19AFCC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1337,54 +1371,55 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>